<commit_message>
Updated defaults and user-modified tester file
</commit_message>
<xml_diff>
--- a/www/defaults_rema_fip.xlsx
+++ b/www/defaults_rema_fip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juancarlosvillasenorderbez/GitHub/AppCosteo/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDAFF0B-6319-414A-AF99-739B816AD88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F48052-4140-3540-A4DC-BBBB8A45CB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{B4A74D70-26A4-944B-8A76-86924F5026A1}"/>
   </bookViews>
@@ -11428,8 +11428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB6DD39-1495-0F4F-A3DB-1A099904BD7D}">
   <dimension ref="A1:Q477"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>